<commit_message>
Edit Pattani post location
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -3381,8 +3381,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F1164"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="A1151" workbookViewId="0">
-      <selection activeCell="F1162" sqref="F1162"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="A1127" workbookViewId="0">
+      <selection activeCell="F1133" sqref="F1133"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -25907,10 +25907,10 @@
         <v>965</v>
       </c>
       <c r="E1126" s="1">
-        <v>6.6433831999999997</v>
+        <v>6.6754850000000001</v>
       </c>
       <c r="F1126" s="1">
-        <v>101.1843887</v>
+        <v>101.151025</v>
       </c>
     </row>
     <row r="1127" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
@@ -25927,10 +25927,10 @@
         <v>966</v>
       </c>
       <c r="E1127" s="1">
-        <v>6.8016240000000003</v>
+        <v>6.8437010000000003</v>
       </c>
       <c r="F1127" s="1">
-        <v>101.1519275</v>
+        <v>101.177943</v>
       </c>
     </row>
     <row r="1128" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
@@ -25947,10 +25947,10 @@
         <v>967</v>
       </c>
       <c r="E1128" s="1">
-        <v>6.8031936999999996</v>
+        <v>6.8578469999999996</v>
       </c>
       <c r="F1128" s="1">
-        <v>101.5475409</v>
+        <v>101.48952</v>
       </c>
     </row>
     <row r="1129" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
@@ -25967,10 +25967,10 @@
         <v>967</v>
       </c>
       <c r="E1129" s="1">
-        <v>6.7519372000000004</v>
+        <v>6.7514620000000001</v>
       </c>
       <c r="F1129" s="1">
-        <v>101.490712</v>
+        <v>101.485283</v>
       </c>
     </row>
     <row r="1130" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
@@ -25987,10 +25987,10 @@
         <v>968</v>
       </c>
       <c r="E1130" s="1">
-        <v>6.7168672999999997</v>
+        <v>6.7202679999999999</v>
       </c>
       <c r="F1130" s="1">
-        <v>101.41688190000001</v>
+        <v>101.412981</v>
       </c>
     </row>
     <row r="1131" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
@@ -26007,10 +26007,10 @@
         <v>968</v>
       </c>
       <c r="E1131" s="1">
-        <v>6.7519372000000004</v>
+        <v>6.7514620000000001</v>
       </c>
       <c r="F1131" s="1">
-        <v>101.490712</v>
+        <v>101.485283</v>
       </c>
     </row>
     <row r="1132" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
@@ -26027,10 +26027,10 @@
         <v>969</v>
       </c>
       <c r="E1132" s="1">
-        <v>6.6349729000000002</v>
+        <v>6.7202679999999999</v>
       </c>
       <c r="F1132" s="1">
-        <v>101.4479702</v>
+        <v>101.412981</v>
       </c>
     </row>
     <row r="1133" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
@@ -26047,10 +26047,10 @@
         <v>970</v>
       </c>
       <c r="E1133" s="1">
-        <v>6.6759310000000003</v>
+        <v>6.7055239999999996</v>
       </c>
       <c r="F1133" s="1">
-        <v>101.5930268</v>
+        <v>101.61830999999999</v>
       </c>
     </row>
     <row r="1134" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
@@ -26067,10 +26067,10 @@
         <v>970</v>
       </c>
       <c r="E1134" s="1">
-        <v>6.7519372000000004</v>
+        <v>6.7514620000000001</v>
       </c>
       <c r="F1134" s="1">
-        <v>101.490712</v>
+        <v>101.485283</v>
       </c>
     </row>
     <row r="1135" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
@@ -26087,10 +26087,10 @@
         <v>971</v>
       </c>
       <c r="E1135" s="1">
-        <v>6.6479271999999998</v>
+        <v>6.613429</v>
       </c>
       <c r="F1135" s="1">
-        <v>101.6669843</v>
+        <v>101.669015</v>
       </c>
     </row>
     <row r="1136" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
@@ -26107,10 +26107,10 @@
         <v>972</v>
       </c>
       <c r="E1136" s="1">
-        <v>6.8485889999999996</v>
+        <v>6.8625829999999999</v>
       </c>
       <c r="F1136" s="1">
-        <v>101.4112049</v>
+        <v>101.369112</v>
       </c>
     </row>
     <row r="1137" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
@@ -26127,10 +26127,10 @@
         <v>972</v>
       </c>
       <c r="E1137" s="1">
-        <v>6.7519372000000004</v>
+        <v>6.7514620000000001</v>
       </c>
       <c r="F1137" s="1">
-        <v>101.490712</v>
+        <v>101.485283</v>
       </c>
     </row>
     <row r="1138" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
@@ -26147,10 +26147,10 @@
         <v>973</v>
       </c>
       <c r="E1138" s="1">
-        <v>6.6930902000000003</v>
+        <v>6.758667</v>
       </c>
       <c r="F1138" s="1">
-        <v>101.3090737</v>
+        <v>101.293631</v>
       </c>
     </row>
     <row r="1139" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
@@ -26167,10 +26167,10 @@
         <v>974</v>
       </c>
       <c r="E1139" s="1">
-        <v>6.5930213000000002</v>
+        <v>6.5612360000000001</v>
       </c>
       <c r="F1139" s="1">
-        <v>101.5475409</v>
+        <v>101.534651</v>
       </c>
     </row>
     <row r="1140" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
@@ -26187,10 +26187,10 @@
         <v>975</v>
       </c>
       <c r="E1140" s="1">
-        <v>6.6474770000000003</v>
+        <v>6.6754850000000001</v>
       </c>
       <c r="F1140" s="1">
-        <v>101.2353772</v>
+        <v>101.151025</v>
       </c>
     </row>
     <row r="1141" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Edit Chaiyaphum post loacation
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2332" uniqueCount="1005">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4664" uniqueCount="1005">
   <si>
     <t>กรุงเทพมหานคร</t>
   </si>
@@ -3381,8 +3381,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F1164"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="A1127" workbookViewId="0">
-      <selection activeCell="F1133" sqref="F1133"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="A388" workbookViewId="0">
+      <selection activeCell="F391" sqref="F391"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -11207,10 +11207,10 @@
         <v>347</v>
       </c>
       <c r="E391" s="1">
-        <v>15.8675815</v>
+        <v>15.806777</v>
       </c>
       <c r="F391" s="1">
-        <v>102.026135</v>
+        <v>102.029293</v>
       </c>
     </row>
     <row r="392" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
@@ -11227,10 +11227,10 @@
         <v>347</v>
       </c>
       <c r="E392" s="1">
-        <v>15.7021955</v>
+        <v>15.683754</v>
       </c>
       <c r="F392" s="1">
-        <v>102.0946818</v>
+        <v>102.01066</v>
       </c>
     </row>
     <row r="393" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
@@ -11267,10 +11267,10 @@
         <v>349</v>
       </c>
       <c r="E394" s="1">
-        <v>15.9443409</v>
+        <v>15.931618</v>
       </c>
       <c r="F394" s="1">
-        <v>102.30058029999999</v>
+        <v>102.280219</v>
       </c>
     </row>
     <row r="395" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
@@ -11287,10 +11287,10 @@
         <v>350</v>
       </c>
       <c r="E395" s="1">
-        <v>16.2426241</v>
+        <v>16.278825000000001</v>
       </c>
       <c r="F395" s="1">
-        <v>101.9348069</v>
+        <v>101.955924</v>
       </c>
     </row>
     <row r="396" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
@@ -11307,10 +11307,10 @@
         <v>351</v>
       </c>
       <c r="E396" s="1">
-        <v>16.0908333</v>
+        <v>16.082166999999998</v>
       </c>
       <c r="F396" s="1">
-        <v>101.7969444</v>
+        <v>101.803854</v>
       </c>
     </row>
     <row r="397" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
@@ -11327,10 +11327,10 @@
         <v>352</v>
       </c>
       <c r="E397" s="1">
-        <v>15.6006885</v>
+        <v>15.566482000000001</v>
       </c>
       <c r="F397" s="1">
-        <v>101.8435568</v>
+        <v>101.850792</v>
       </c>
     </row>
     <row r="398" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
@@ -11347,10 +11347,10 @@
         <v>352</v>
       </c>
       <c r="E398" s="1">
-        <v>15.5690426</v>
+        <v>15.414806</v>
       </c>
       <c r="F398" s="1">
-        <v>101.8562733</v>
+        <v>101.83433100000001</v>
       </c>
     </row>
     <row r="399" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
@@ -11367,10 +11367,10 @@
         <v>353</v>
       </c>
       <c r="E399" s="1">
-        <v>15.442702000000001</v>
+        <v>15.489515000000001</v>
       </c>
       <c r="F399" s="1">
-        <v>101.688248</v>
+        <v>101.686803</v>
       </c>
     </row>
     <row r="400" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
@@ -11407,10 +11407,10 @@
         <v>354</v>
       </c>
       <c r="E401" s="1">
-        <v>15.7538158</v>
+        <v>15.750667</v>
       </c>
       <c r="F401" s="1">
-        <v>101.7865654</v>
+        <v>101.761933</v>
       </c>
     </row>
     <row r="402" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
@@ -11427,10 +11427,10 @@
         <v>355</v>
       </c>
       <c r="E402" s="1">
-        <v>15.363868</v>
+        <v>15.388782000000001</v>
       </c>
       <c r="F402" s="1">
-        <v>101.460769</v>
+        <v>101.447052</v>
       </c>
     </row>
     <row r="403" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
@@ -11447,10 +11447,10 @@
         <v>356</v>
       </c>
       <c r="E403" s="1">
-        <v>16.3763389</v>
+        <v>16.369183</v>
       </c>
       <c r="F403" s="1">
-        <v>102.1287289</v>
+        <v>102.135346</v>
       </c>
     </row>
     <row r="404" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
@@ -11467,10 +11467,10 @@
         <v>357</v>
       </c>
       <c r="E404" s="1">
-        <v>16.3793702</v>
+        <v>16.405733999999999</v>
       </c>
       <c r="F404" s="1">
-        <v>102.3692982</v>
+        <v>102.34308799999999</v>
       </c>
     </row>
     <row r="405" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
@@ -11487,10 +11487,10 @@
         <v>358</v>
       </c>
       <c r="E405" s="1">
-        <v>16.134407499999998</v>
+        <v>16.109124999999999</v>
       </c>
       <c r="F405" s="1">
-        <v>102.20902239999999</v>
+        <v>102.25751700000001</v>
       </c>
     </row>
     <row r="406" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
@@ -11507,10 +11507,10 @@
         <v>359</v>
       </c>
       <c r="E406" s="1">
-        <v>16.600500799999999</v>
+        <v>16.613334999999999</v>
       </c>
       <c r="F406" s="1">
-        <v>101.9040309</v>
+        <v>101.918847</v>
       </c>
     </row>
     <row r="407" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
@@ -11527,10 +11527,10 @@
         <v>360</v>
       </c>
       <c r="E407" s="1">
-        <v>16.0168745</v>
+        <v>15.908200000000001</v>
       </c>
       <c r="F407" s="1">
-        <v>101.4112049</v>
+        <v>101.41925000000001</v>
       </c>
     </row>
     <row r="408" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Edit Ranong post location 2019 10
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4664" uniqueCount="1005">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2332" uniqueCount="1005">
   <si>
     <t>กรุงเทพมหานคร</t>
   </si>
@@ -3381,8 +3381,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F1164"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="A388" workbookViewId="0">
-      <selection activeCell="F391" sqref="F391"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="A1022" workbookViewId="0">
+      <selection activeCell="F1044" sqref="F1044"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -24167,10 +24167,10 @@
         <v>901</v>
       </c>
       <c r="E1039" s="1">
-        <v>9.85914</v>
+        <v>9.9720393000000005</v>
       </c>
       <c r="F1039" s="1">
-        <v>98.594081399999993</v>
+        <v>98.640088500000005</v>
       </c>
     </row>
     <row r="1040" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
@@ -24267,10 +24267,10 @@
         <v>905</v>
       </c>
       <c r="E1044" s="1">
-        <v>9.4210452</v>
+        <v>9.5846699999999991</v>
       </c>
       <c r="F1044" s="1">
-        <v>98.462298700000005</v>
+        <v>98.591121000000001</v>
       </c>
     </row>
     <row r="1045" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">

</xml_diff>